<commit_message>
Add cashflow analysis with EUR conversion and 2H period calculations
</commit_message>
<xml_diff>
--- a/data/excel/NBIM_Cashflow.xlsx
+++ b/data/excel/NBIM_Cashflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hobao\NBIM\NBIM\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85BB3999-ECA0-455E-BF67-D6E44AC0B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE466AC8-9091-46B7-9C42-A3D761177E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2287" yWindow="322" windowWidth="14401" windowHeight="7336" xr2:uid="{13A3FEC5-12B0-4249-A00A-3D4E1572A2F3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{13A3FEC5-12B0-4249-A00A-3D4E1572A2F3}"/>
   </bookViews>
   <sheets>
     <sheet name="cashflow-template" sheetId="1" r:id="rId1"/>
@@ -60,21 +60,6 @@
     <t>Period</t>
   </si>
   <si>
-    <t>Receipts Interest</t>
-  </si>
-  <si>
-    <t>Receipts Dividends</t>
-  </si>
-  <si>
-    <t>New Investments</t>
-  </si>
-  <si>
-    <t>Development Assets</t>
-  </si>
-  <si>
-    <t>Receipts_Ongoing Operations</t>
-  </si>
-  <si>
     <t>Net_Investment CF</t>
   </si>
   <si>
@@ -88,6 +73,21 @@
   </si>
   <si>
     <t>Full year</t>
+  </si>
+  <si>
+    <t>Receipts_Interest</t>
+  </si>
+  <si>
+    <t>Receipts_Dividends</t>
+  </si>
+  <si>
+    <t>New_Investments</t>
+  </si>
+  <si>
+    <t>Development_Assets</t>
+  </si>
+  <si>
+    <t>Repayments_loan</t>
   </si>
 </sst>
 </file>
@@ -951,9 +951,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3046D840-E063-4E6F-A481-38B8091FA4F8}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -963,28 +974,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -992,7 +1003,7 @@
         <v>2021</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1021,7 +1032,7 @@
         <v>2021</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>80</v>
@@ -1050,7 +1061,7 @@
         <v>2022</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>96</v>
@@ -1082,7 +1093,7 @@
         <v>2022</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>162</v>
@@ -1111,7 +1122,7 @@
         <v>2023</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>143</v>
@@ -1143,7 +1154,7 @@
         <v>2023</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>397</v>
@@ -1175,7 +1186,7 @@
         <v>2024</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>199</v>
@@ -1207,7 +1218,7 @@
         <v>2024</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>407</v>
@@ -1239,7 +1250,7 @@
         <v>2025</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>247</v>

</xml_diff>